<commit_message>
Propuesta y Oferta economica
</commit_message>
<xml_diff>
--- a/Bom.xlsx
+++ b/Bom.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\universidad\DRLW\ProyectoDRLW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego23p\Documents\U\9no\DRLW\ProyectoDRLW\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868C11A9-6A97-4A81-8F9A-B01CE1782FE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7590"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -210,7 +219,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$$-240A]\ * #,##0_-;\-[$$-240A]\ * #,##0_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
@@ -482,167 +491,167 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -958,11 +967,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -970,172 +979,172 @@
     <col min="6" max="8" width="9.140625" customWidth="1" outlineLevel="1"/>
     <col min="9" max="9" width="53" customWidth="1" outlineLevel="1"/>
     <col min="10" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="6.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="6.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:14" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="3:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43" t="s">
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43" t="s">
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="43"/>
-      <c r="L3" s="44" t="s">
+      <c r="K3" s="34"/>
+      <c r="L3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="45"/>
-      <c r="N3" s="7" t="s">
+      <c r="M3" s="36"/>
+      <c r="N3" s="57" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="3:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="8"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="58"/>
     </row>
     <row r="5" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="41" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="48">
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="33">
         <v>4</v>
       </c>
-      <c r="K5" s="48"/>
-      <c r="L5" s="49">
+      <c r="K5" s="33"/>
+      <c r="L5" s="23">
         <v>508569</v>
       </c>
-      <c r="M5" s="50"/>
+      <c r="M5" s="24"/>
       <c r="N5" s="4">
         <f>L5/(1-0.25)</f>
         <v>678092</v>
       </c>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="52"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="26"/>
       <c r="N6" s="4"/>
     </row>
     <row r="7" spans="3:14" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="54"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="28"/>
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="41" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="48">
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="33">
         <v>4</v>
       </c>
-      <c r="K8" s="48"/>
-      <c r="L8" s="49">
+      <c r="K8" s="33"/>
+      <c r="L8" s="23">
         <v>2817500</v>
       </c>
-      <c r="M8" s="50"/>
+      <c r="M8" s="24"/>
       <c r="N8" s="4">
         <f t="shared" ref="N8" si="0">L8/(1-0.25)</f>
         <v>3756666.6666666665</v>
       </c>
     </row>
     <row r="9" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="52"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="26"/>
       <c r="N9" s="4"/>
     </row>
     <row r="10" spans="3:14" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="54"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="28"/>
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="41" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="48">
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="33">
         <v>8</v>
       </c>
-      <c r="K11" s="48"/>
+      <c r="K11" s="33"/>
       <c r="L11" s="4">
         <v>84000</v>
       </c>
@@ -1146,49 +1155,49 @@
       </c>
     </row>
     <row r="12" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="48"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
     </row>
     <row r="13" spans="3:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
     <row r="14" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="41" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="48">
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="33">
         <v>8</v>
       </c>
-      <c r="K14" s="48"/>
+      <c r="K14" s="33"/>
       <c r="L14" s="4">
         <v>1500000</v>
       </c>
@@ -1199,222 +1208,246 @@
       </c>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="48"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
     </row>
     <row r="16" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="48"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
     </row>
     <row r="17" spans="3:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="35" t="s">
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="25">
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="13">
         <v>4</v>
       </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="29">
+      <c r="K17" s="14"/>
+      <c r="L17" s="17">
         <v>473428</v>
       </c>
-      <c r="M17" s="30"/>
-      <c r="N17" s="5">
+      <c r="M17" s="18"/>
+      <c r="N17" s="21">
         <f>L17/(1-0.25)</f>
         <v>631237.33333333337</v>
       </c>
     </row>
     <row r="18" spans="3:16" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="22"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="41" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="48">
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="33">
         <v>1</v>
       </c>
-      <c r="K19" s="48"/>
+      <c r="K19" s="33"/>
       <c r="L19" s="4">
         <v>10000000</v>
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4">
-        <f t="shared" ref="N19" si="3">L19/(1-0.25)</f>
-        <v>13333333.333333334</v>
+        <f>L19</f>
+        <v>10000000</v>
       </c>
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="35" t="s">
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="25">
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="13">
         <v>1</v>
       </c>
-      <c r="K22" s="26"/>
-      <c r="L22" s="29">
+      <c r="K22" s="14"/>
+      <c r="L22" s="17">
         <v>3000000</v>
       </c>
-      <c r="M22" s="30"/>
-      <c r="N22" s="5">
-        <f>L22/(1-0.25)</f>
-        <v>4000000</v>
+      <c r="M22" s="18"/>
+      <c r="N22" s="21">
+        <f>L22</f>
+        <v>3000000</v>
       </c>
     </row>
     <row r="23" spans="3:16" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="22"/>
     </row>
     <row r="24" spans="3:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="15" t="s">
+      <c r="D24" s="42"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="55" t="s">
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="K24" s="56"/>
-      <c r="L24" s="57">
-        <f>(L5*$J5)+(L8*$J8)+(L11*$J11)+(L14*$J14)+(L17*$J17)+(L19*$J19)+(L22*$J22)</f>
-        <v>40869988</v>
-      </c>
-      <c r="M24" s="58"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="31">
+        <f>(L5*$J5)+(L8*$J8)+(L11*$J11)+(L14*$J14)+(L17*$J17)</f>
+        <v>27869988</v>
+      </c>
+      <c r="M24" s="32"/>
       <c r="N24" s="3">
-        <f>(N5*$J5)+(N8*$J8)+(N11*$J11)+(N14*$J14)+(N17*$J17)+(N19*$J19)+(N22*$J22)</f>
-        <v>54493317.333333336</v>
+        <f>(N5*$J5)+(N8*$J8)+(N11*$J11)+(N14*$J14)+(N17*$J17)+(N19*$J19)</f>
+        <v>47159984</v>
       </c>
     </row>
     <row r="25" spans="3:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C25" s="12"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="21" t="s">
+      <c r="C25" s="44"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="22"/>
-      <c r="L25" s="23">
-        <f>(L5*$J5)+(L8*$J8)+(L11*$J11)+(L17*$J17)+(L19*$J19)+(L22*$J22)</f>
-        <v>28869988</v>
-      </c>
-      <c r="M25" s="24"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="55">
+        <f>(L5*$J5)+(L8*$J8)+(L11*$J11)+(L17*$J17)</f>
+        <v>15869988</v>
+      </c>
+      <c r="M25" s="56"/>
       <c r="N25" s="2">
-        <f>(N5*$J5)+(N8*$J8)+(N11*$J11)+(N17*$J17)+(N19*$J19)+(N22*$J22)</f>
-        <v>38493317.333333328</v>
+        <f>(N5*$J5)+(N8*$J8)+(N11*$J11)+(N17*$J17)+(N19*$J19)</f>
+        <v>31159983.999999996</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="N19:N21"/>
-    <mergeCell ref="C22:E23"/>
-    <mergeCell ref="F22:I23"/>
-    <mergeCell ref="J22:K23"/>
-    <mergeCell ref="L22:M23"/>
-    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="N14:N16"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="N5:N7"/>
+    <mergeCell ref="N8:N10"/>
+    <mergeCell ref="N11:N13"/>
+    <mergeCell ref="C24:E25"/>
+    <mergeCell ref="F24:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="J17:K18"/>
+    <mergeCell ref="L17:M18"/>
+    <mergeCell ref="C17:E18"/>
+    <mergeCell ref="F17:I18"/>
+    <mergeCell ref="C19:E21"/>
+    <mergeCell ref="F19:I21"/>
+    <mergeCell ref="C11:E13"/>
+    <mergeCell ref="C14:E16"/>
+    <mergeCell ref="F5:I7"/>
+    <mergeCell ref="F8:I10"/>
+    <mergeCell ref="F11:I13"/>
+    <mergeCell ref="F14:I16"/>
+    <mergeCell ref="C8:E10"/>
+    <mergeCell ref="C3:E4"/>
+    <mergeCell ref="F3:I4"/>
+    <mergeCell ref="J3:K4"/>
+    <mergeCell ref="L3:M4"/>
+    <mergeCell ref="C5:E7"/>
+    <mergeCell ref="J5:K7"/>
+    <mergeCell ref="L5:M7"/>
     <mergeCell ref="L8:M10"/>
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="L24:M24"/>
@@ -1425,36 +1458,12 @@
     <mergeCell ref="J8:K10"/>
     <mergeCell ref="J19:K21"/>
     <mergeCell ref="L19:M21"/>
-    <mergeCell ref="C3:E4"/>
-    <mergeCell ref="F3:I4"/>
-    <mergeCell ref="J3:K4"/>
-    <mergeCell ref="L3:M4"/>
-    <mergeCell ref="C5:E7"/>
-    <mergeCell ref="J5:K7"/>
-    <mergeCell ref="L5:M7"/>
-    <mergeCell ref="C11:E13"/>
-    <mergeCell ref="C14:E16"/>
-    <mergeCell ref="F5:I7"/>
-    <mergeCell ref="F8:I10"/>
-    <mergeCell ref="F11:I13"/>
-    <mergeCell ref="F14:I16"/>
-    <mergeCell ref="C8:E10"/>
-    <mergeCell ref="C24:E25"/>
-    <mergeCell ref="F24:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="J17:K18"/>
-    <mergeCell ref="L17:M18"/>
-    <mergeCell ref="C17:E18"/>
-    <mergeCell ref="F17:I18"/>
-    <mergeCell ref="C19:E21"/>
-    <mergeCell ref="F19:I21"/>
-    <mergeCell ref="N14:N16"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="N5:N7"/>
-    <mergeCell ref="N8:N10"/>
-    <mergeCell ref="N11:N13"/>
+    <mergeCell ref="N19:N21"/>
+    <mergeCell ref="C22:E23"/>
+    <mergeCell ref="F22:I23"/>
+    <mergeCell ref="J22:K23"/>
+    <mergeCell ref="L22:M23"/>
+    <mergeCell ref="N22:N23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>